<commit_message>
adding import data notebook
</commit_message>
<xml_diff>
--- a/data/ccy-date.xlsx
+++ b/data/ccy-date.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\rmccrickerd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmccrickerd\Desktop\jdheston\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28:K28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1020,7 +1020,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>6.2720000000000002</v>
+        <v>6.27</v>
       </c>
       <c r="C4">
         <v>0.7</v>
@@ -1055,7 +1055,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>6.99</v>
       </c>
       <c r="C5">
         <v>0.7</v>
@@ -1090,7 +1090,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>8.9239999999999995</v>
+        <v>8.8849999999999998</v>
       </c>
       <c r="C6">
         <v>0.75</v>
@@ -1125,10 +1125,10 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>9.673</v>
+        <v>9.61</v>
       </c>
       <c r="C7">
-        <v>0.65100000000000002</v>
+        <v>0.65</v>
       </c>
       <c r="D7">
         <v>9.2089999999999996</v>

</xml_diff>